<commit_message>
US-#22 Update excel format
</commit_message>
<xml_diff>
--- a/Documentation/Estimate cost.xlsx
+++ b/Documentation/Estimate cost.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USN_Study\Autonomous-Car-CHEBB\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FDC84E1-7D8A-4313-9078-71E2B62E2159}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{006F3D73-D929-4493-B5C9-BDE6B4B8C7DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{905A884C-9D4C-4A7C-B630-7EA46FA9D602}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>Three point estimates</t>
   </si>
@@ -96,6 +96,18 @@
   </si>
   <si>
     <t>(OC + 4*MC+PC)/6</t>
+  </si>
+  <si>
+    <t>software</t>
+  </si>
+  <si>
+    <t>sharelatex/visual sudio</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Budget</t>
   </si>
 </sst>
 </file>
@@ -111,15 +123,51 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -127,19 +175,229 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -188,7 +446,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -484,253 +742,331 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB7AB3F4-702F-4AA3-8E67-CA9AA0FDE8F6}">
-  <dimension ref="C5:K13"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="11.42578125" style="1"/>
-    <col min="4" max="11" width="17" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="11.42578125" style="1"/>
+    <col min="2" max="2" width="22.85546875" style="1" customWidth="1"/>
+    <col min="3" max="9" width="17" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C5" s="3" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="4"/>
     </row>
-    <row r="6" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="D6" s="1" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="C2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="D2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="E2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="F2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="G2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="H2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="I2" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C7" s="1" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="B3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="1">
+      <c r="C3" s="14">
         <v>4</v>
       </c>
-      <c r="F7" s="1">
+      <c r="D3" s="15">
         <v>12000</v>
       </c>
-      <c r="G7" s="1">
+      <c r="E3" s="15">
         <v>13500</v>
       </c>
-      <c r="H7" s="1">
+      <c r="F3" s="15">
         <v>15000</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="G3" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="J7" s="1">
-        <f>(F7+G7*4+H7)/6</f>
+      <c r="H3" s="15">
+        <f>(D3+E3*4+F3)/6</f>
         <v>13500</v>
       </c>
-      <c r="K7" s="1">
-        <f>E7*J7</f>
+      <c r="I3" s="16">
+        <f>C3*H3</f>
         <v>54000</v>
       </c>
     </row>
-    <row r="8" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C8" s="1" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="B4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="1">
+      <c r="C4" s="17">
         <v>1</v>
       </c>
-      <c r="F8" s="1">
+      <c r="D4" s="18">
         <v>3560</v>
       </c>
-      <c r="G8" s="1">
+      <c r="E4" s="18">
         <v>4560</v>
       </c>
-      <c r="H8" s="1">
+      <c r="F4" s="18">
         <v>6000</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="G4" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="J8" s="1">
-        <f>(F8+G8*4+H8)/6</f>
+      <c r="H4" s="18">
+        <f>(D4+E4*4+F4)/6</f>
         <v>4633.333333333333</v>
       </c>
-      <c r="K8" s="1">
-        <f>E8*J8</f>
+      <c r="I4" s="19">
+        <f>C4*H4</f>
         <v>4633.333333333333</v>
       </c>
     </row>
-    <row r="9" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C9" s="1" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="B5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="1">
+      <c r="C5" s="17">
         <v>1</v>
       </c>
-      <c r="F9" s="1">
+      <c r="D5" s="18">
         <v>250</v>
       </c>
-      <c r="G9" s="1">
+      <c r="E5" s="18">
         <v>350</v>
       </c>
-      <c r="H9" s="1">
+      <c r="F5" s="18">
         <v>400</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="G5" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="J9" s="1">
-        <f t="shared" ref="J9:J12" si="0">(F9+G9*4+H9)/6</f>
+      <c r="H5" s="18">
+        <f t="shared" ref="H5:H10" si="0">(D5+E5*4+F5)/6</f>
         <v>341.66666666666669</v>
       </c>
-      <c r="K9" s="1">
-        <f t="shared" ref="K9:K12" si="1">E9*J9</f>
+      <c r="I5" s="19">
+        <f t="shared" ref="I5:I9" si="1">C5*H5</f>
         <v>341.66666666666669</v>
       </c>
     </row>
-    <row r="10" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C10" s="1" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="B6" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="1">
+      <c r="C6" s="17">
         <v>1</v>
       </c>
-      <c r="F10" s="1">
+      <c r="D6" s="18">
         <v>700</v>
       </c>
-      <c r="G10" s="1">
+      <c r="E6" s="18">
         <v>1000</v>
       </c>
-      <c r="H10" s="1">
+      <c r="F6" s="18">
         <v>2000</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="G6" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="J10" s="1">
+      <c r="H6" s="18">
         <f t="shared" si="0"/>
         <v>1116.6666666666667</v>
       </c>
-      <c r="K10" s="1">
+      <c r="I6" s="19">
         <f t="shared" si="1"/>
         <v>1116.6666666666667</v>
       </c>
     </row>
-    <row r="11" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C11" s="1" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="B7" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="1">
+      <c r="C7" s="17">
         <v>1</v>
       </c>
-      <c r="F11" s="1">
+      <c r="D7" s="18">
         <v>350</v>
       </c>
-      <c r="G11" s="1">
+      <c r="E7" s="18">
         <v>900</v>
       </c>
-      <c r="H11" s="1">
+      <c r="F7" s="18">
         <v>2000</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="G7" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="J11" s="1">
+      <c r="H7" s="18">
         <f t="shared" si="0"/>
         <v>991.66666666666663</v>
       </c>
-      <c r="K11" s="1">
+      <c r="I7" s="19">
         <f t="shared" si="1"/>
         <v>991.66666666666663</v>
       </c>
     </row>
-    <row r="12" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C12" s="1" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="B8" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="1">
+      <c r="C8" s="17">
         <v>2</v>
       </c>
-      <c r="F12" s="1">
+      <c r="D8" s="18">
         <v>250</v>
       </c>
-      <c r="G12" s="1">
+      <c r="E8" s="18">
         <v>300</v>
       </c>
-      <c r="H12" s="1">
+      <c r="F8" s="18">
         <v>450</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="G8" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="J12" s="1">
+      <c r="H8" s="18">
         <f t="shared" si="0"/>
         <v>316.66666666666669</v>
       </c>
-      <c r="K12" s="1">
+      <c r="I8" s="19">
         <f t="shared" si="1"/>
         <v>633.33333333333337</v>
       </c>
     </row>
-    <row r="13" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="K13" s="1">
-        <f>SUM(K7:K12)</f>
-        <v>61716.666666666664</v>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="20">
+        <v>4</v>
+      </c>
+      <c r="D9" s="21">
+        <f>880+14400</f>
+        <v>15280</v>
+      </c>
+      <c r="E9" s="21">
+        <f>880+16000</f>
+        <v>16880</v>
+      </c>
+      <c r="F9" s="21">
+        <f>1760+24000</f>
+        <v>25760</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="21">
+        <f t="shared" si="0"/>
+        <v>18093.333333333332</v>
+      </c>
+      <c r="I9" s="22">
+        <f t="shared" si="1"/>
+        <v>72373.333333333328</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="24"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="27">
+        <f>$C$3*D3+$C$4*D4+$C$5*D5+$C$6*D6+$C$7*D7+$C$8*D8+$C$9*D9</f>
+        <v>114480</v>
+      </c>
+      <c r="E10" s="27">
+        <f t="shared" ref="E10:F10" si="2">$C$3*E3+$C$4*E4+$C$5*E5+$C$6*E6+$C$7*E7+$C$8*E8+$C$9*E9</f>
+        <v>128930</v>
+      </c>
+      <c r="F10" s="27">
+        <f t="shared" si="2"/>
+        <v>174340</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="29">
+        <f t="shared" si="0"/>
+        <v>134090</v>
+      </c>
+      <c r="I10" s="26">
+        <f>SUM(I3:I9)</f>
+        <v>134090</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="32"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" s="31">
+        <f>I10*1.15</f>
+        <v>154203.5</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C5:K5"/>
+  <mergeCells count="3">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:G11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>